<commit_message>
#136 fix nested horizontal ranges
</commit_message>
<xml_diff>
--- a/tests/Templates/HorizontalRange.xlsx
+++ b/tests/Templates/HorizontalRange.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\asr\ClosedXML.Report\tests\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="20700" windowHeight="11760"/>
   </bookViews>
@@ -43,8 +48,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -75,7 +80,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -104,19 +109,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -136,40 +128,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="3" tint="0.39994506668294322"/>
@@ -180,6 +200,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -228,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,9 +283,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,6 +318,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -469,46 +494,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -516,7 +541,7 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:D4">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>ISEVEN(B$3)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Bugfix/#136 nested horiz rng (#221)
* #136 fix nested horizontal ranges
</commit_message>
<xml_diff>
--- a/tests/Templates/HorizontalRange.xlsx
+++ b/tests/Templates/HorizontalRange.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\asr\ClosedXML.Report\tests\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="20700" windowHeight="11760"/>
   </bookViews>
@@ -43,8 +48,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -75,7 +80,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -104,19 +109,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -136,40 +128,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="3" tint="0.39994506668294322"/>
@@ -180,6 +200,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -228,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,9 +283,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,6 +318,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -469,46 +494,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -516,7 +541,7 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:D4">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>ISEVEN(B$3)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>